<commit_message>
added the link to the inventory app service
</commit_message>
<xml_diff>
--- a/resources_list.xlsx
+++ b/resources_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhin\Documents\AZURE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2AFB5F6-96AF-4BB3-A79D-9034B64866D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C494228A-74F7-4954-A871-81D2E15A8F34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{5BA57FA7-8E92-4029-A248-24F9453A1440}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Resources Helper List:</t>
   </si>
@@ -93,6 +85,9 @@
   </si>
   <si>
     <t>Front Door URL</t>
+  </si>
+  <si>
+    <t>my-inventory-abhinav.azurewebsites.net</t>
   </si>
 </sst>
 </file>
@@ -573,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485C0861-5CBA-4053-BC6E-30C1C65B6942}">
-  <dimension ref="A12:A36"/>
+  <dimension ref="A12:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,67 +600,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -697,21 +695,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x010100898F1BA822CA7A4C9E1EECD7B51A5D33" ma:contentTypeVersion="12" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="292e6f1fa068b859e132649c2a3d4505">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1b4877c-7963-4fff-ba17-2b68774beed0" xmlns:ns4="3b2c9cc2-5cae-4dfd-ac5b-cf044e8522f6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a51703ec1358e54068ea21a055be5de" ns3:_="" ns4:_="">
     <xsd:import namespace="e1b4877c-7963-4fff-ba17-2b68774beed0"/>
@@ -928,32 +911,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C70B530C-897A-4399-9B70-5D017B8BAB92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3b2c9cc2-5cae-4dfd-ac5b-cf044e8522f6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="e1b4877c-7963-4fff-ba17-2b68774beed0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A747CE42-258D-45DA-89E7-DE516928E2F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10A24DD0-6E43-439F-8DA8-5B3CDFECFD79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -970,4 +943,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A747CE42-258D-45DA-89E7-DE516928E2F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C70B530C-897A-4399-9B70-5D017B8BAB92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3b2c9cc2-5cae-4dfd-ac5b-cf044e8522f6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="e1b4877c-7963-4fff-ba17-2b68774beed0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>